<commit_message>
Scripting DPLKINV001-001 and DPLKINV001-002, Update Excel DPLKINV001-001 until DPLKINV001-007, AND update Preparation
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV001-001 - Setup Portofolio Investasi - General Tambah, Ubah, View Detil & Hapus Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV001-001 - Setup Portofolio Investasi - General Tambah, Ubah, View Detil & Hapus Data.xlsx
@@ -8,29 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAFFBE7-5D64-44C9-AE0D-FF89B5D3B0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCFA1E7-7B06-4FAF-B222-9DA764D2EE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DPLKINV001" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
   <si>
     <t>SIDEBAR_MENU</t>
   </si>
@@ -158,68 +148,41 @@
     <t>Pasar Modal Edit Test</t>
   </si>
   <si>
-    <t>View :
-1. Klik icon Lihat Detail pada baris yang dituju</t>
-  </si>
-  <si>
-    <t>Tambah :
-1. Akses menu setup
-2. Klik tombol tambah
-3. Masukkan data
-4. Klik tombol Simpan</t>
-  </si>
-  <si>
-    <t>Ubah :
-1. Klik icon Ubah pada baris yang dituju
-2. Sesuaikan data yang ingin diubah
-3. Klik Simpan</t>
-  </si>
-  <si>
-    <t>Hapus :
-1. Klik icon Hapus pada baris yang dituju
-2. Klik tombol Ya, yakin!</t>
-  </si>
-  <si>
-    <t>Menampilkan Log Tambah Data</t>
-  </si>
-  <si>
-    <t>Administration</t>
-  </si>
-  <si>
-    <t>Laporan</t>
-  </si>
-  <si>
-    <t>Log Audit Trail</t>
-  </si>
-  <si>
-    <t>Create</t>
-  </si>
-  <si>
-    <t>Update</t>
-  </si>
-  <si>
-    <t>Log Web Tambah Data :
-1. Akses menu Laporan -&gt; Log Audit Trail
-2. Klik tombol View Detail</t>
-  </si>
-  <si>
-    <t>Log Web Update Data:
-1. Akses menu Laporan -&gt; Log Audit Trail
-2. Klik tombol View Detail</t>
-  </si>
-  <si>
-    <t>Menampilkan Log Update Data</t>
-  </si>
-  <si>
-    <t>Log Web Delete Data:
-1. Akses menu Laporan -&gt; Log Audit Trail
-2. Klik tombol View Detail</t>
-  </si>
-  <si>
-    <t>Menampilkan Log Delete Data</t>
-  </si>
-  <si>
-    <t>Delete</t>
+    <t>Tambah Setup Portofolio</t>
+  </si>
+  <si>
+    <t>View Setup Portofolio</t>
+  </si>
+  <si>
+    <t>Ubah Setup Portofolio</t>
+  </si>
+  <si>
+    <t>Hapus Setup Portofolio</t>
+  </si>
+  <si>
+    <t>PREPARATION</t>
+  </si>
+  <si>
+    <t>Username : Putri;
+Password : bni1234/;
+Porto Id : PM018;
+Porto Nama : Pasar Modal Test;
+Inv Id : PM - Pasar Modal;
+Kode : PM;
+No Urut : 181;
+Prefix Surat : P12345678;
+Porto Id OJK : P87654321;
+Keterangan : INV.SET.001</t>
+  </si>
+  <si>
+    <t>Username : Putri;
+Password : bni1234/;
+Porto Id : PM018</t>
+  </si>
+  <si>
+    <t>Username : Putri;
+Password : bni1234/;
+Porto Nama : Pasar Modal Edit Test</t>
   </si>
 </sst>
 </file>
@@ -280,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -304,9 +267,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -614,11 +574,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
-  <dimension ref="A1:U9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="99" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,25 +587,25 @@
     <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
-    <col min="15" max="16" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="1"/>
-    <col min="21" max="21" width="12" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="6" width="32.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="1" customWidth="1"/>
+    <col min="16" max="17" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="1"/>
+    <col min="22" max="22" width="12" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -662,55 +622,58 @@
         <v>5</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -721,59 +684,62 @@
         <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4"/>
+      <c r="M2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="8">
+      <c r="Q2" s="8">
         <v>181</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="U2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="V2" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -784,48 +750,43 @@
         <v>19</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="9" t="str">
-        <f ca="1">TEXT(TODAY(),"dd/mm/yyyy")</f>
-        <v>24/11/2022</v>
-      </c>
+      <c r="I3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="4"/>
       <c r="M3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="N3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="8"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="7"/>
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
     </row>
-    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -836,40 +797,46 @@
         <v>19</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4"/>
+      <c r="M4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="8"/>
+      <c r="N4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="P4" s="7"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="4"/>
+      <c r="T4" s="8"/>
       <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
     </row>
-    <row r="5" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -880,189 +847,52 @@
         <v>19</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4"/>
+      <c r="M5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="8" t="s">
-        <v>41</v>
-      </c>
       <c r="N5" s="5"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="8"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="7"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
-      <c r="T5" s="4"/>
+      <c r="T5" s="8"/>
       <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
     </row>
-    <row r="6" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="9" t="str">
-        <f ca="1">TEXT(TODAY(),"dd/mm/yyyy")</f>
-        <v>24/11/2022</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-    </row>
-    <row r="8" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="9" t="str">
-        <f ca="1">TEXT(TODAY(),"dd/mm/yyyy")</f>
-        <v>24/11/2022</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Fixing DPLKINV001-001 and Scripting DPLKINV001-002 until DPLKINV001-004
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV001-001 - Setup Portofolio Investasi - General Tambah, Ubah, View Detil & Hapus Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV001-001 - Setup Portofolio Investasi - General Tambah, Ubah, View Detil & Hapus Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCFA1E7-7B06-4FAF-B222-9DA764D2EE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F0DFF1-5467-481E-B545-4910E07BF49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="49">
   <si>
     <t>SIDEBAR_MENU</t>
   </si>
@@ -28,9 +28,6 @@
     <t>SIDEBAR_SUBMENU</t>
   </si>
   <si>
-    <t>SIDEBAR_SUBMENU_SUBMENU</t>
-  </si>
-  <si>
     <t>RUN</t>
   </si>
   <si>
@@ -52,30 +49,6 @@
     <t>PASSWORD</t>
   </si>
   <si>
-    <t>TEXT1</t>
-  </si>
-  <si>
-    <t>TEXT2</t>
-  </si>
-  <si>
-    <t>TEXT3</t>
-  </si>
-  <si>
-    <t>TEXT4</t>
-  </si>
-  <si>
-    <t>TEXT5</t>
-  </si>
-  <si>
-    <t>TEXT6</t>
-  </si>
-  <si>
-    <t>TEXT7</t>
-  </si>
-  <si>
-    <t>TEXT8</t>
-  </si>
-  <si>
     <t>INV001-001</t>
   </si>
   <si>
@@ -131,12 +104,6 @@
   </si>
   <si>
     <t>Hapus Data Dapat dilakukan dengan baik</t>
-  </si>
-  <si>
-    <t>TEXT9</t>
-  </si>
-  <si>
-    <t>TEXT10</t>
   </si>
   <si>
     <t>0 : Pending Register</t>
@@ -183,6 +150,36 @@
     <t>Username : Putri;
 Password : bni1234/;
 Porto Nama : Pasar Modal Edit Test</t>
+  </si>
+  <si>
+    <t>PORTO_ID</t>
+  </si>
+  <si>
+    <t>PORTO_NAMA</t>
+  </si>
+  <si>
+    <t>INV_ID</t>
+  </si>
+  <si>
+    <t>KODE</t>
+  </si>
+  <si>
+    <t>NO_URUT</t>
+  </si>
+  <si>
+    <t>PREFIX_SURAT</t>
+  </si>
+  <si>
+    <t>PORTO_ID_OJK</t>
+  </si>
+  <si>
+    <t>KETERANGAN</t>
+  </si>
+  <si>
+    <t>STATUS_REGISTER</t>
+  </si>
+  <si>
+    <t>KETERANGAN_REGISTER</t>
   </si>
 </sst>
 </file>
@@ -575,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,45 +590,46 @@
     <col min="9" max="9" width="17.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="1" customWidth="1"/>
-    <col min="16" max="17" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="1"/>
-    <col min="22" max="22" width="12" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="12" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>0</v>
@@ -640,256 +638,249 @@
         <v>1</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="D2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="J2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="L2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="M2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="8">
+        <v>181</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="V1" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="150" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="8">
-        <v>181</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="G3" s="5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="7"/>
+        <v>16</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="5"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
+      <c r="T3" s="4"/>
       <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
     </row>
-    <row r="4" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="7"/>
+        <v>16</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
+      <c r="T4" s="4"/>
       <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
     </row>
-    <row r="5" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
+      <c r="T5" s="4"/>
       <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>

</xml_diff>